<commit_message>
lineups working. just need player with ball now
</commit_message>
<xml_diff>
--- a/extractor.xlsx
+++ b/extractor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\GitHub\2k21Extractor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\GitHub\2k22Extractor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BA5C64-A5EB-4625-A682-D0FA4EDE0C13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1379E7-A75A-4679-8162-830DC54E1D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5415" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38460" yWindow="9345" windowWidth="28740" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="player stats" sheetId="1" r:id="rId1"/>
@@ -583,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H3:H21"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,10 +595,10 @@
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>63</v>
       </c>
@@ -606,7 +606,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -619,15 +619,19 @@
       <c r="H2">
         <v>23296</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2">
+        <f>H2+32</f>
+        <v>23328</v>
+      </c>
+      <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" t="str">
-        <f t="shared" ref="J2:J23" si="0">"new Offset("""&amp;G2&amp;""","&amp;H2&amp;","&amp;I2</f>
-        <v>new Offset("SecondsPlayed",23296,StatDataType.Float),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="str">
+        <f>"new Offset("""&amp;G2&amp;""","&amp;I2&amp;","&amp;J2</f>
+        <v>new Offset("SecondsPlayed",23328,StatDataType.Float),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -643,15 +647,19 @@
       <c r="H3">
         <v>22224</v>
       </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("Points",22224,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <f t="shared" ref="I3:I24" si="0">H3+32</f>
+        <v>22256</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K23" si="1">"new Offset("""&amp;G3&amp;""","&amp;I3&amp;","&amp;J3</f>
+        <v>new Offset("Points",22256,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -667,15 +675,19 @@
       <c r="H4">
         <v>23258</v>
       </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("DefRebounds",23258,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>23290</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("DefRebounds",23290,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -691,15 +703,19 @@
       <c r="H5">
         <v>23288</v>
       </c>
-      <c r="I5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("Assists",23288,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>23320</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("Assists",23320,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -715,15 +731,19 @@
       <c r="H6">
         <v>23280</v>
       </c>
-      <c r="I6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("Steals",23280,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>23312</v>
+      </c>
+      <c r="J6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("Steals",23312,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -739,15 +759,19 @@
       <c r="H7">
         <v>23282</v>
       </c>
-      <c r="I7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("Blocks",23282,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>23314</v>
+      </c>
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("Blocks",23314,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -763,15 +787,19 @@
       <c r="H8">
         <v>23292</v>
       </c>
-      <c r="I8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("Turnovers",23292,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>23324</v>
+      </c>
+      <c r="J8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("Turnovers",23324,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -787,15 +815,19 @@
       <c r="H9">
         <v>22232</v>
       </c>
-      <c r="I9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("TwoPM",22232,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>22264</v>
+      </c>
+      <c r="J9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("TwoPM",22264,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -811,15 +843,19 @@
       <c r="H10">
         <v>22234</v>
       </c>
-      <c r="I10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("TwoPA",22234,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>22266</v>
+      </c>
+      <c r="J10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("TwoPA",22266,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -835,15 +871,19 @@
       <c r="H11">
         <v>22236</v>
       </c>
-      <c r="I11" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("ThreePM",22236,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>22268</v>
+      </c>
+      <c r="J11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("ThreePM",22268,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -859,15 +899,19 @@
       <c r="H12">
         <v>22238</v>
       </c>
-      <c r="I12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("ThreePA",22238,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>22270</v>
+      </c>
+      <c r="J12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("ThreePA",22270,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -883,15 +927,19 @@
       <c r="H13">
         <v>22228</v>
       </c>
-      <c r="I13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("FTM",22228,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>22260</v>
+      </c>
+      <c r="J13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("FTM",22260,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -907,15 +955,19 @@
       <c r="H14">
         <v>22230</v>
       </c>
-      <c r="I14" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("FTA",22230,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>22262</v>
+      </c>
+      <c r="J14" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("FTA",22262,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -931,15 +983,19 @@
       <c r="H15">
         <v>23256</v>
       </c>
-      <c r="I15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("OffRebounds",23256,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>23288</v>
+      </c>
+      <c r="J15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("OffRebounds",23288,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -955,15 +1011,19 @@
       <c r="H16">
         <v>23284</v>
       </c>
-      <c r="I16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("Fouls",23284,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>23316</v>
+      </c>
+      <c r="J16" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("Fouls",23316,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -976,15 +1036,19 @@
       <c r="H17">
         <v>23304</v>
       </c>
-      <c r="I17" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("PlusMinus",23304,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>23336</v>
+      </c>
+      <c r="J17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("PlusMinus",23336,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1000,15 +1064,19 @@
       <c r="H18">
         <v>23290</v>
       </c>
-      <c r="I18" t="s">
-        <v>23</v>
-      </c>
-      <c r="J18" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("PointsAssisted",23290,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>23322</v>
+      </c>
+      <c r="J18" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("PointsAssisted",23322,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1018,15 +1086,19 @@
       <c r="H19">
         <v>22248</v>
       </c>
-      <c r="I19" t="s">
-        <v>23</v>
-      </c>
-      <c r="J19" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("PointsInPaint",22248,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>22280</v>
+      </c>
+      <c r="J19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("PointsInPaint",22280,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1036,15 +1108,19 @@
       <c r="H20">
         <v>22268</v>
       </c>
-      <c r="I20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("SecondChancePoints",22268,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>22300</v>
+      </c>
+      <c r="J20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("SecondChancePoints",22300,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1054,15 +1130,19 @@
       <c r="H21">
         <v>22266</v>
       </c>
-      <c r="I21" t="s">
-        <v>23</v>
-      </c>
-      <c r="J21" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("FastBreakPoints",22266,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>22298</v>
+      </c>
+      <c r="J21" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("FastBreakPoints",22298,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1072,15 +1152,19 @@
       <c r="H22">
         <v>22250</v>
       </c>
-      <c r="I22" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("PointsOffTurnovers",22250,StatDataType.TwoByteInt),</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>22282</v>
+      </c>
+      <c r="J22" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("PointsOffTurnovers",22282,StatDataType.TwoByteInt),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1090,15 +1174,19 @@
       <c r="H23">
         <v>23284</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>23316</v>
+      </c>
+      <c r="J23" t="s">
         <v>24</v>
       </c>
-      <c r="J23" t="str">
-        <f t="shared" si="0"/>
-        <v>new Offset("Dunks",23284,StatDataType.TwoByteInt)</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v>new Offset("Dunks",23316,StatDataType.TwoByteInt)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>62</v>
       </c>
@@ -1119,7 +1207,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>